<commit_message>
Changed formatting on a couple problems
</commit_message>
<xml_diff>
--- a/matlab_attempt/Excel problems/Basics questions.xlsx
+++ b/matlab_attempt/Excel problems/Basics questions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Google Drive\Quant Methods for Biology\Adaptive\Sections\2. Basics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Documents\Github\QMB-Problem-Maker\matlab_attempt\Excel problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2B5777E0-031E-41A1-B824-E899327083B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{845E9CE6-CFEC-4CFF-8B4C-ABDACEE48547}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="8925" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="415">
   <si>
     <t>questionText</t>
   </si>
@@ -854,9 +854,6 @@
     <t>sym2</t>
   </si>
   <si>
-    <t>if strcmp('OP1','less'), result2 = NUM4*result1 - NUM3; sym2 = '-'; else, result2 = NUM4*result1 + NUM3; sym2 = '+'; end</t>
-  </si>
-  <si>
     <t>if strcmp('OP1','sum'), result1 = NUM1 + NUM2;  sym1 = '+'; elseif strcmp('OP1','product'), result1 = NUM1 * NUM2; sym1 = '*'; else, result1 = NUM1-NUM2; sym1 = '-'; end</t>
   </si>
   <si>
@@ -911,9 +908,6 @@
     <t>opword</t>
   </si>
   <si>
-    <t>if strcmp('OP1','less'), sol_str = 'Since subtraction is not commutative, there is only one correct way to write this: ANS1'; else; sol_str = 'Since addition is commutative, there are two ways you can write this: ANS1 and ANS3'; end</t>
-  </si>
-  <si>
     <t>if strcmp('OP1','less'), opword = 'subtract'; else, opword = 'add'; end</t>
   </si>
   <si>
@@ -921,12 +915,6 @@
   </si>
   <si>
     <t>The important thing to remember here is Order of Operations. The phrase "NUM1 OP1 than NUM2 times $XX/$" implies you need to multiply $XX/$ by the value NUM2 and then OPWORD NUM1. SOL_STR.</t>
-  </si>
-  <si>
-    <t>if strcmp('OP1','less'), answers = {'$YY = NUM2 * XX - NUM1/$','$YY = NUM1 * YY - NUM2/$','$YY = NUM1 - XX * NUM2/$','$YY = NUM2 - XX * NUM1/$', 'None of these'}; correctness = {'TRUE','FALSE','FALSE','FALSE','FALSE'}; end</t>
-  </si>
-  <si>
-    <t>if strcmp('OP1','more'), answers = {'$YY = NUM2 * XX + NUM1/$','$YY = NUM1 * YY + NUM2/$','$YY = NUM1 + XX * NUM2/$','$YY = NUM2 + XX * NUM1/$', 'None of these'}; correctness = {'TRUE','FALSE','TRUE','FALSE','FALSE'}; end</t>
   </si>
   <si>
     <t>randsample(1:10,2)</t>
@@ -1093,9 +1081,6 @@
     <t>incorrect{4}</t>
   </si>
   <si>
-    <t xml:space="preserve">Store the OP1 of NUM1 and NUM2 to a variable named $XX/$. Store NUM3 OP2 than NUM4 times $XX/$ to a variable named $YY/$. What number is stored to the variable with the OP3 value of $XX/$ and $YY/$? </t>
-  </si>
-  <si>
     <t>variable5</t>
   </si>
   <si>
@@ -1236,12 +1221,81 @@
   <si>
     <t>B7</t>
   </si>
+  <si>
+    <t>FMT</t>
+  </si>
+  <si>
+    <t>MS21</t>
+  </si>
+  <si>
+    <t>MS12</t>
+  </si>
+  <si>
+    <t>SM12</t>
+  </si>
+  <si>
+    <t>SM21</t>
+  </si>
+  <si>
+    <t>MA21</t>
+  </si>
+  <si>
+    <t>MA12</t>
+  </si>
+  <si>
+    <t>AM12</t>
+  </si>
+  <si>
+    <t>AM21</t>
+  </si>
+  <si>
+    <t>if strcmp('OP1','less'), answers = {'MS21','MS12','SM12','SM21', 'None of these'}; correctness = {'TRUE','FALSE','FALSE','FALSE','FALSE'}; end</t>
+  </si>
+  <si>
+    <t>if strcmp('OP1','more'), answers = {'MA21','MA12','AM12','AM21', 'None of these'}; correctness = {'TRUE','FALSE','FALSE','FALSE','FALSE'}; end</t>
+  </si>
+  <si>
+    <t>['YY' ' = %d %c ' 'XX' ' %c %d']</t>
+  </si>
+  <si>
+    <t>['$' sprintf('FMT',NUM2,'+','*',NUM1) '/$']</t>
+  </si>
+  <si>
+    <t>['$' sprintf('FMT',NUM1,'+','*',NUM2) '/$']</t>
+  </si>
+  <si>
+    <t>['$' sprintf('FMT',NUM2,'*','-',NUM1) '/$']</t>
+  </si>
+  <si>
+    <t>['$' sprintf('FMT',NUM1,'*','-',NUM2) '/$']</t>
+  </si>
+  <si>
+    <t>['$' sprintf('FMT',NUM1,'-','*',NUM2) '/$']</t>
+  </si>
+  <si>
+    <t>['$' sprintf('FMT',NUM2,'-','*',NUM1) '/$']</t>
+  </si>
+  <si>
+    <t>['$' sprintf('FMT',NUM2,'*','+',NUM1) '/$']</t>
+  </si>
+  <si>
+    <t>['$' sprintf('FMT',NUM1,'*','+',NUM2) '/$']</t>
+  </si>
+  <si>
+    <t>if strcmp('OP1','less'), sol_str = ['Since subtraction is not commutative, there is only one correct way to write this: ' 'ANS1']; else; sol_str = ['Since addition is commutative, there are two ways you can write this: ' 'ANS1' ' and ' 'ANS3']; end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store the OP1 of NUM1 and NUM2 to a variable named $XX/$. Store NUM3 OP2 than NUM4 times $XX/$ to a variable named $YY/$. What number is stored to the variable with the OP3 value between $XX/$ and $YY/$? </t>
+  </si>
+  <si>
+    <t>if strcmp('OP2','less'), result2 = NUM4*result1 - NUM3; sym2 = '-'; else, result2 = NUM4*result1 + NUM3; sym2 = '+'; end</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1266,6 +1320,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Hack"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1297,7 +1357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1337,6 +1397,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1770,7 +1842,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E7" s="17" t="b">
         <v>1</v>
@@ -1824,10 +1896,10 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="17" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -1979,7 +2051,7 @@
         <v>80</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E22" s="17" t="b">
         <v>1</v>
@@ -2010,10 +2082,10 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="17" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
@@ -2205,7 +2277,7 @@
         <v>80</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E40" s="17" t="b">
         <v>1</v>
@@ -2288,10 +2360,10 @@
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="17"/>
       <c r="B47" s="17" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
@@ -2373,7 +2445,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -2438,10 +2510,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C9" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2512,7 +2584,7 @@
         <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
@@ -2566,10 +2638,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C22" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2625,7 +2697,7 @@
         <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E27" t="b">
         <v>1</v>
@@ -2693,10 +2765,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C34" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F34" s="1"/>
     </row>
@@ -2768,7 +2840,7 @@
         <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E40" t="b">
         <v>1</v>
@@ -2824,10 +2896,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
+        <v>366</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>371</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2919,7 +2991,7 @@
         <v>33</v>
       </c>
       <c r="D53" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E53" t="b">
         <v>1</v>
@@ -2969,10 +3041,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -3030,7 +3102,7 @@
         <v>29</v>
       </c>
       <c r="D63" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E63" t="b">
         <v>1</v>
@@ -3105,10 +3177,10 @@
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -3173,7 +3245,7 @@
         <v>47</v>
       </c>
       <c r="D75" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E75" t="b">
         <v>1</v>
@@ -3246,10 +3318,10 @@
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C82" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -3296,7 +3368,7 @@
         <v>46</v>
       </c>
       <c r="D86" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E86" t="b">
         <v>1</v>
@@ -3342,7 +3414,7 @@
         <v>49</v>
       </c>
       <c r="D89" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E89" t="b">
         <v>1</v>
@@ -3397,10 +3469,10 @@
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C94" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3448,7 +3520,7 @@
         <v>46</v>
       </c>
       <c r="D98" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E98" t="b">
         <v>1</v>
@@ -3530,10 +3602,10 @@
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C105" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F105" s="1"/>
     </row>
@@ -3577,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -3592,7 +3664,7 @@
         <v>1</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E110" s="1" t="b">
         <v>1</v>
@@ -3626,10 +3698,10 @@
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
@@ -3679,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D117" s="8"/>
       <c r="E117" s="1"/>
@@ -3694,7 +3766,7 @@
         <v>3</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E118" s="1" t="b">
         <v>1</v>
@@ -3728,10 +3800,10 @@
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -3781,7 +3853,7 @@
         <v>0</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D125" s="8"/>
       <c r="E125" s="1"/>
@@ -3796,7 +3868,7 @@
         <v>2</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E126" s="1" t="b">
         <v>1</v>
@@ -3830,10 +3902,10 @@
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -3940,7 +4012,7 @@
         <v>121</v>
       </c>
       <c r="D138" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E138" t="b">
         <v>1</v>
@@ -3972,10 +4044,10 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C142" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -4090,7 +4162,7 @@
         <v>125</v>
       </c>
       <c r="D153" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E153" t="b">
         <v>1</v>
@@ -4122,10 +4194,10 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C157" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4240,7 +4312,7 @@
         <v>126</v>
       </c>
       <c r="D168" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E168" t="b">
         <v>1</v>
@@ -4272,10 +4344,10 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C172" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4311,7 +4383,7 @@
         <v>0</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4552,7 +4624,7 @@
         <v>80</v>
       </c>
       <c r="D197" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E197" t="b">
         <v>1</v>
@@ -4653,7 +4725,7 @@
         <v>0</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -4894,7 +4966,7 @@
         <v>80</v>
       </c>
       <c r="D228" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E228" t="b">
         <v>1</v>
@@ -4995,7 +5067,7 @@
         <v>0</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -5224,7 +5296,7 @@
         <v>80</v>
       </c>
       <c r="D258" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E258" t="b">
         <v>1</v>
@@ -5325,7 +5397,7 @@
         <v>0</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -5369,7 +5441,7 @@
         <v>251</v>
       </c>
       <c r="D272" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -5391,7 +5463,7 @@
         <v>136</v>
       </c>
       <c r="D274" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -5413,7 +5485,7 @@
         <v>136</v>
       </c>
       <c r="D276" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
@@ -5424,7 +5496,7 @@
         <v>136</v>
       </c>
       <c r="D277" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -5555,7 +5627,7 @@
         <v>80</v>
       </c>
       <c r="D288" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E288" t="b">
         <v>1</v>
@@ -5618,7 +5690,7 @@
         <v>25</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -5650,13 +5722,13 @@
     </row>
     <row r="298" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B298" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C298" s="14" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -5664,10 +5736,10 @@
         <v>75</v>
       </c>
       <c r="C299" s="11" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D299" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -5689,7 +5761,7 @@
         <v>80</v>
       </c>
       <c r="D301" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -5701,7 +5773,7 @@
         <v>81</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -5712,7 +5784,7 @@
         <v>136</v>
       </c>
       <c r="D303" s="6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -5723,7 +5795,7 @@
         <v>136</v>
       </c>
       <c r="D304" s="6" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -5742,10 +5814,10 @@
         <v>75</v>
       </c>
       <c r="C306" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D306" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
@@ -5753,10 +5825,10 @@
         <v>75</v>
       </c>
       <c r="C307" s="6" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D307" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
@@ -5767,10 +5839,10 @@
         <v>80</v>
       </c>
       <c r="D308" s="6" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E308" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
@@ -5781,10 +5853,10 @@
         <v>81</v>
       </c>
       <c r="D309" s="6" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E309" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
@@ -5818,7 +5890,7 @@
         <v>25</v>
       </c>
       <c r="C313" s="13" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D313" s="10"/>
       <c r="E313" s="10"/>
@@ -5836,13 +5908,13 @@
     </row>
     <row r="315" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B315" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
@@ -5853,7 +5925,7 @@
         <v>101</v>
       </c>
       <c r="D316" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
@@ -5861,7 +5933,7 @@
         <v>2</v>
       </c>
       <c r="C317" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E317" t="b">
         <v>0</v>
@@ -5872,10 +5944,10 @@
         <v>2</v>
       </c>
       <c r="C318" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D318" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E318" t="b">
         <v>1</v>
@@ -5886,7 +5958,7 @@
         <v>2</v>
       </c>
       <c r="C319" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E319" t="b">
         <v>0</v>
@@ -5897,7 +5969,7 @@
         <v>2</v>
       </c>
       <c r="C320" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E320" t="b">
         <v>0</v>
@@ -5932,7 +6004,7 @@
         <v>25</v>
       </c>
       <c r="C324" s="13" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="325" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5948,13 +6020,13 @@
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B326" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C326" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
@@ -5962,10 +6034,10 @@
         <v>75</v>
       </c>
       <c r="C327" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D327" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
@@ -5976,7 +6048,7 @@
         <v>117</v>
       </c>
       <c r="D328" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
@@ -5984,7 +6056,7 @@
         <v>75</v>
       </c>
       <c r="C329" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D329">
         <v>0.2</v>
@@ -5998,7 +6070,7 @@
         <v>136</v>
       </c>
       <c r="D330" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
@@ -6006,10 +6078,10 @@
         <v>75</v>
       </c>
       <c r="C331" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D331" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
@@ -6031,7 +6103,7 @@
         <v>81</v>
       </c>
       <c r="D333" s="6" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -6042,7 +6114,7 @@
         <v>82</v>
       </c>
       <c r="D334" s="6" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
@@ -6053,7 +6125,7 @@
         <v>106</v>
       </c>
       <c r="D335" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
@@ -6064,7 +6136,7 @@
         <v>104</v>
       </c>
       <c r="D336" s="6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
@@ -6075,7 +6147,7 @@
         <v>80</v>
       </c>
       <c r="D337" s="16" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="E337" t="b">
         <v>1</v>
@@ -6146,7 +6218,7 @@
         <v>25</v>
       </c>
       <c r="C344" s="13" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="345" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6162,13 +6234,13 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B346" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C346" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
@@ -6176,10 +6248,10 @@
         <v>75</v>
       </c>
       <c r="C347" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D347" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
@@ -6190,7 +6262,7 @@
         <v>117</v>
       </c>
       <c r="D348" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
@@ -6198,7 +6270,7 @@
         <v>75</v>
       </c>
       <c r="C349" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D349">
         <v>0.2</v>
@@ -6212,7 +6284,7 @@
         <v>136</v>
       </c>
       <c r="D350" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
@@ -6220,10 +6292,10 @@
         <v>75</v>
       </c>
       <c r="C351" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D351" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
@@ -6245,7 +6317,7 @@
         <v>81</v>
       </c>
       <c r="D353" s="6" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
@@ -6256,7 +6328,7 @@
         <v>82</v>
       </c>
       <c r="D354" s="6" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
@@ -6267,7 +6339,7 @@
         <v>106</v>
       </c>
       <c r="D355" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
@@ -6278,7 +6350,7 @@
         <v>104</v>
       </c>
       <c r="D356" s="6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
@@ -6289,7 +6361,7 @@
         <v>80</v>
       </c>
       <c r="D357" s="16" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="E357" t="b">
         <v>1</v>
@@ -6360,7 +6432,7 @@
         <v>25</v>
       </c>
       <c r="C364" s="13" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="365" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6376,13 +6448,13 @@
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B366" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C366" s="11" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
@@ -6393,7 +6465,7 @@
         <v>117</v>
       </c>
       <c r="D367" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
@@ -6404,7 +6476,7 @@
         <v>136</v>
       </c>
       <c r="D368" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="369" spans="2:5" x14ac:dyDescent="0.25">
@@ -6412,10 +6484,10 @@
         <v>75</v>
       </c>
       <c r="C369" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D369" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="370" spans="2:5" x14ac:dyDescent="0.25">
@@ -6426,7 +6498,7 @@
         <v>136</v>
       </c>
       <c r="D370" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="371" spans="2:5" x14ac:dyDescent="0.25">
@@ -6434,10 +6506,10 @@
         <v>75</v>
       </c>
       <c r="C371" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="D371" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="372" spans="2:5" x14ac:dyDescent="0.25">
@@ -6448,7 +6520,7 @@
         <v>136</v>
       </c>
       <c r="D372" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="373" spans="2:5" x14ac:dyDescent="0.25">
@@ -6456,10 +6528,10 @@
         <v>75</v>
       </c>
       <c r="C373" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D373" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="374" spans="2:5" x14ac:dyDescent="0.25">
@@ -6467,10 +6539,10 @@
         <v>75</v>
       </c>
       <c r="C374" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D374" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="375" spans="2:5" x14ac:dyDescent="0.25">
@@ -6478,10 +6550,10 @@
         <v>75</v>
       </c>
       <c r="C375" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D375" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="376" spans="2:5" x14ac:dyDescent="0.25">
@@ -6492,7 +6564,7 @@
         <v>80</v>
       </c>
       <c r="D376" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="377" spans="2:5" x14ac:dyDescent="0.25">
@@ -6503,7 +6575,7 @@
         <v>81</v>
       </c>
       <c r="D377" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="378" spans="2:5" x14ac:dyDescent="0.25">
@@ -6514,7 +6586,7 @@
         <v>82</v>
       </c>
       <c r="D378" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="379" spans="2:5" x14ac:dyDescent="0.25">
@@ -6525,7 +6597,7 @@
         <v>136</v>
       </c>
       <c r="D379" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="380" spans="2:5" x14ac:dyDescent="0.25">
@@ -6533,7 +6605,7 @@
         <v>75</v>
       </c>
       <c r="C380" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D380" t="s">
         <v>2</v>
@@ -6547,10 +6619,10 @@
         <v>80</v>
       </c>
       <c r="D381" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E381" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="382" spans="2:5" x14ac:dyDescent="0.25">
@@ -6561,10 +6633,10 @@
         <v>81</v>
       </c>
       <c r="D382" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E382" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="383" spans="2:5" x14ac:dyDescent="0.25">
@@ -6575,10 +6647,10 @@
         <v>82</v>
       </c>
       <c r="D383" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E383" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="384" spans="2:5" x14ac:dyDescent="0.25">
@@ -6613,7 +6685,7 @@
         <v>25</v>
       </c>
       <c r="C387" s="13" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="388" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6626,13 +6698,13 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B389" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C389" s="11" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
@@ -6643,7 +6715,7 @@
         <v>117</v>
       </c>
       <c r="D390" s="15" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
@@ -6651,10 +6723,10 @@
         <v>75</v>
       </c>
       <c r="C391" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D391" s="15" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
@@ -6665,7 +6737,7 @@
         <v>136</v>
       </c>
       <c r="D392" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
@@ -6673,10 +6745,10 @@
         <v>75</v>
       </c>
       <c r="C393" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="D393" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
@@ -6687,7 +6759,7 @@
         <v>136</v>
       </c>
       <c r="D394" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
@@ -6695,10 +6767,10 @@
         <v>75</v>
       </c>
       <c r="C395" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D395" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
@@ -6706,10 +6778,10 @@
         <v>75</v>
       </c>
       <c r="C396" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D396" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
@@ -6717,10 +6789,10 @@
         <v>75</v>
       </c>
       <c r="C397" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D397" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
@@ -6731,7 +6803,7 @@
         <v>80</v>
       </c>
       <c r="D398" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
@@ -6742,7 +6814,7 @@
         <v>81</v>
       </c>
       <c r="D399" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
@@ -6753,7 +6825,7 @@
         <v>82</v>
       </c>
       <c r="D400" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="401" spans="2:5" x14ac:dyDescent="0.25">
@@ -6764,7 +6836,7 @@
         <v>136</v>
       </c>
       <c r="D401" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="402" spans="2:5" x14ac:dyDescent="0.25">
@@ -6772,7 +6844,7 @@
         <v>75</v>
       </c>
       <c r="C402" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D402" t="s">
         <v>2</v>
@@ -6786,10 +6858,10 @@
         <v>80</v>
       </c>
       <c r="D403" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E403" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="404" spans="2:5" x14ac:dyDescent="0.25">
@@ -6800,10 +6872,10 @@
         <v>81</v>
       </c>
       <c r="D404" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E404" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="405" spans="2:5" x14ac:dyDescent="0.25">
@@ -6814,10 +6886,10 @@
         <v>82</v>
       </c>
       <c r="D405" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E405" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="406" spans="2:5" x14ac:dyDescent="0.25">
@@ -6852,7 +6924,7 @@
         <v>25</v>
       </c>
       <c r="C409" s="13" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="410" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6949,7 +7021,7 @@
         <v>184</v>
       </c>
       <c r="D6" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -7164,7 +7236,7 @@
         <v>184</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -7402,7 +7474,7 @@
         <v>184</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E44" t="b">
         <v>1</v>
@@ -7594,7 +7666,7 @@
         <v>80</v>
       </c>
       <c r="D60" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E60" t="b">
         <v>1</v>
@@ -7740,7 +7812,7 @@
         <v>80</v>
       </c>
       <c r="D74" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E74" t="b">
         <v>1</v>
@@ -24340,7 +24412,7 @@
         <v>80</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E92" s="10" t="b">
         <v>1</v>
@@ -40908,7 +40980,7 @@
         <v>80</v>
       </c>
       <c r="D108" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E108" t="b">
         <v>1</v>
@@ -41039,7 +41111,7 @@
         <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -41149,7 +41221,7 @@
         <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
@@ -41396,7 +41468,7 @@
         <v>80</v>
       </c>
       <c r="D39" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E39" t="b">
         <v>1</v>
@@ -41622,7 +41694,7 @@
         <v>80</v>
       </c>
       <c r="D60" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E60" t="b">
         <v>1</v>
@@ -41674,7 +41746,7 @@
         <v>7</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -41687,950 +41759,1239 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828A1C0C-F645-470C-80A4-C9B344E57619}">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="C1" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="24" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="21" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="21" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="E4" s="21"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="21" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="21" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="21" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="21" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="E8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="21" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="21" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="21" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="E18" s="21"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="E19" s="21"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E20" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+    </row>
+    <row r="22" spans="1:5" ht="192" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="21">
+        <v>2</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+    </row>
+    <row r="27" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="21"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="21"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
+      <c r="B30" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="21"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+      <c r="B31" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="E31" s="21"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="21"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" s="21"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="E34" s="21"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="E35" s="21"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="E36" s="21"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>394</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="E37" s="21"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>395</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="E38" s="21"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="E39" s="21"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>410</v>
+      </c>
+      <c r="E40" s="21"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>398</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>411</v>
+      </c>
+      <c r="E41" s="21"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>399</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="E42" s="21"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="E43" s="21"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="21"/>
+      <c r="B44" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="E44" s="21"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="E45" s="21"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="E46" s="21"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="21"/>
+      <c r="B47" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="E47" s="21"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="21"/>
+      <c r="B48" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="21" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="E48" s="21"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
+      <c r="B49" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C13" t="s">
-        <v>258</v>
-      </c>
-      <c r="D13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="C49" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="E49" s="21"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C14" t="s">
-        <v>264</v>
-      </c>
-      <c r="D14" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="C50" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="E50" s="21"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C51" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="E51" s="21"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="B52" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="E52" s="21"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+      <c r="B53" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="D15" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="D53" s="21" t="s">
+        <v>412</v>
+      </c>
+      <c r="E53" s="21"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+      <c r="B54" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C16" t="s">
-        <v>259</v>
-      </c>
-      <c r="D16" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C54" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="E54" s="21"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="21"/>
+      <c r="B55" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C17" t="s">
-        <v>269</v>
-      </c>
-      <c r="D17" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="C55" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="E55" s="21"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="21"/>
+      <c r="B56" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C56" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="E56" s="21"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="21"/>
+      <c r="B57" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="E57" s="21"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+      <c r="B58" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="E58" s="21"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+      <c r="B59" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>278</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="E59" s="21"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="21"/>
+      <c r="B60" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="21"/>
+      <c r="B61" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="21"/>
+      <c r="B62" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E62" s="21" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="21"/>
+      <c r="B63" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E63" s="21" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="21"/>
+      <c r="B64" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E64" s="21" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="21"/>
+      <c r="B65" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+    </row>
+    <row r="66" spans="1:5" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="21"/>
+      <c r="B66" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="21"/>
+      <c r="B67" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="21"/>
+      <c r="B68" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="21"/>
+      <c r="B69" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="21">
+        <v>2</v>
+      </c>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="25"/>
+      <c r="B70" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
+    </row>
+    <row r="71" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A71" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="B71" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="21"/>
+      <c r="B72" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="D18" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="D72" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="E72" s="21"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="21"/>
+      <c r="B73" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C19" t="s">
-        <v>184</v>
-      </c>
-      <c r="D19" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C73" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="D73" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="E73" s="21"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="21"/>
+      <c r="B74" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C74" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="E74" s="21"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="21"/>
+      <c r="B75" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C75" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D75" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="E75" s="21"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="21"/>
+      <c r="B76" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D76" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="E76" s="21"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="21"/>
+      <c r="B77" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C77" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D77" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="E77" s="21"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="21"/>
+      <c r="B78" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C78" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D78" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="E78" s="21"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+      <c r="B79" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C79" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="D79" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="E79" s="21"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="21"/>
+      <c r="B80" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C80" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="D80" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="E80" s="21"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="21"/>
+      <c r="B81" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C81" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="D81" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="E81" s="21"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="21"/>
+      <c r="B82" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C82" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="E82" s="21"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="21"/>
+      <c r="B83" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C83" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="D83" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="E83" s="21"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="21"/>
+      <c r="B84" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C84" s="23" t="s">
+        <v>301</v>
+      </c>
+      <c r="D84" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="E84" s="21"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="21"/>
+      <c r="B85" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C20" t="s">
-        <v>184</v>
-      </c>
-      <c r="D20" t="s">
-        <v>396</v>
-      </c>
-      <c r="E20" t="b">
+      <c r="C85" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D85" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E85" s="21" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="21"/>
+      <c r="B86" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D86" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E86" s="21" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="21"/>
+      <c r="B87" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D87" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E87" s="21" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="21"/>
+      <c r="B88" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C88" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E88" s="21" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="21"/>
+      <c r="B89" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="21"/>
+      <c r="B90" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" s="21"/>
+      <c r="E90" s="21"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="21"/>
+      <c r="B91" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>301</v>
+      </c>
+      <c r="D91" s="21"/>
+      <c r="E91" s="21"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="21"/>
+      <c r="B92" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C92" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="D92" s="21"/>
+      <c r="E92" s="21"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="21"/>
+      <c r="B93" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>191</v>
-      </c>
-      <c r="C23" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="21"/>
+      <c r="B94" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C25">
+      <c r="C94" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
+      <c r="D94" s="21"/>
+      <c r="E94" s="21"/>
+    </row>
+    <row r="95" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="21"/>
+      <c r="B95" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>249</v>
-      </c>
-      <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D31" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" t="s">
-        <v>254</v>
-      </c>
-      <c r="D34" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" t="s">
-        <v>136</v>
-      </c>
-      <c r="D35" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" t="s">
-        <v>136</v>
-      </c>
-      <c r="D37" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" t="s">
-        <v>288</v>
-      </c>
-      <c r="D38" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" t="s">
-        <v>80</v>
-      </c>
-      <c r="D39" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" t="s">
-        <v>82</v>
-      </c>
-      <c r="D41" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>75</v>
-      </c>
-      <c r="C42" t="s">
-        <v>106</v>
-      </c>
-      <c r="D42" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" t="s">
-        <v>136</v>
-      </c>
-      <c r="D44" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" t="s">
-        <v>144</v>
-      </c>
-      <c r="D45" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" t="s">
-        <v>278</v>
-      </c>
-      <c r="D46" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>75</v>
-      </c>
-      <c r="C47" t="s">
-        <v>282</v>
-      </c>
-      <c r="D47" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" t="s">
-        <v>281</v>
-      </c>
-      <c r="D48" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" t="s">
-        <v>280</v>
-      </c>
-      <c r="D49" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>75</v>
-      </c>
-      <c r="C50" t="s">
-        <v>279</v>
-      </c>
-      <c r="D50" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>2</v>
-      </c>
-      <c r="C51" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51" t="s">
-        <v>396</v>
-      </c>
-      <c r="E51" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" t="s">
-        <v>81</v>
-      </c>
-      <c r="D52" t="s">
-        <v>396</v>
-      </c>
-      <c r="E52" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>2</v>
-      </c>
-      <c r="C53" t="s">
-        <v>82</v>
-      </c>
-      <c r="D53" t="s">
-        <v>396</v>
-      </c>
-      <c r="E53" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" t="s">
-        <v>106</v>
-      </c>
-      <c r="D54" t="s">
-        <v>396</v>
-      </c>
-      <c r="E54" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>2</v>
-      </c>
-      <c r="C55" t="s">
-        <v>104</v>
-      </c>
-      <c r="D55" t="s">
-        <v>396</v>
-      </c>
-      <c r="E55" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>191</v>
-      </c>
-      <c r="C58" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-    </row>
-    <row r="62" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>297</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D63" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="D64" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D65" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D67" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D68" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D69" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="D70" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C71" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="D71" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="D72" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C73" s="11" t="s">
+      <c r="C95" s="25" t="s">
         <v>303</v>
       </c>
-      <c r="D73" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="D74" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="D75" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D76" t="s">
-        <v>396</v>
-      </c>
-      <c r="E76" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C77" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D77" t="s">
-        <v>396</v>
-      </c>
-      <c r="E77" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D78" t="s">
-        <v>396</v>
-      </c>
-      <c r="E78" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D79" t="s">
-        <v>396</v>
-      </c>
-      <c r="E79" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D80" t="s">
-        <v>396</v>
-      </c>
-      <c r="E80" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>3</v>
-      </c>
-      <c r="C81" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>25</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>191</v>
-      </c>
-      <c r="C83" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>6</v>
-      </c>
-      <c r="C85">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D86" s="3"/>
+      <c r="D95" s="25"/>
+      <c r="E95" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>